<commit_message>
saving graphs in excel
</commit_message>
<xml_diff>
--- a/PicturesToSubmit/ErrorData.xlsx
+++ b/PicturesToSubmit/ErrorData.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1720" yWindow="0" windowWidth="24880" windowHeight="14740" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1720" yWindow="0" windowWidth="24880" windowHeight="14740" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ErrorVsMinPoints" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Naive Bayes vs Regression" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,14 +21,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>numDiscretizations</t>
   </si>
   <si>
-    <t>discretizations</t>
-  </si>
-  <si>
     <t>10, 20, 30</t>
   </si>
   <si>
@@ -47,6 +45,36 @@
   </si>
   <si>
     <t>10,20,30,40</t>
+  </si>
+  <si>
+    <t>Discretization Points</t>
+  </si>
+  <si>
+    <t>Feature Space</t>
+  </si>
+  <si>
+    <t>Test Error</t>
+  </si>
+  <si>
+    <t>Linear</t>
+  </si>
+  <si>
+    <t>Quadratic (55 features)</t>
+  </si>
+  <si>
+    <t>Quadratic (300 features)</t>
+  </si>
+  <si>
+    <t>Naïve Bayes</t>
+  </si>
+  <si>
+    <t>Number of Features</t>
+  </si>
+  <si>
+    <t>Num. Quantiles</t>
+  </si>
+  <si>
+    <t>Regression</t>
   </si>
 </sst>
 </file>
@@ -95,8 +123,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -109,15 +157,35 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -182,7 +250,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$7</c:f>
+              <c:f>Sheet1!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -191,18 +259,18 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln w="63500"/>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$6:$G$6</c:f>
+              <c:f>Sheet1!$B$5:$G$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
                 <c:pt idx="1">
                   <c:v>5.0</c:v>
                 </c:pt>
@@ -223,27 +291,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$G$7</c:f>
+              <c:f>Sheet1!$B$6:$G$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.655475</c:v>
-                </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.401061</c:v>
+                  <c:v>0.594177</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.30592</c:v>
+                  <c:v>0.404771</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.215207</c:v>
+                  <c:v>0.272377</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.170984</c:v>
+                  <c:v>0.202245</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.160544</c:v>
+                  <c:v>0.188836</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -255,7 +320,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$8</c:f>
+              <c:f>Sheet1!$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -264,18 +329,18 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln w="63500"/>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$6:$G$6</c:f>
+              <c:f>Sheet1!$B$5:$G$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
                 <c:pt idx="1">
                   <c:v>5.0</c:v>
                 </c:pt>
@@ -296,27 +361,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$8:$G$8</c:f>
+              <c:f>Sheet1!$B$7:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.710744</c:v>
-                </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.372809</c:v>
+                  <c:v>0.550219</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.279838</c:v>
+                  <c:v>0.375987</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.207859</c:v>
+                  <c:v>0.265187</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.170132</c:v>
+                  <c:v>0.203362</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.168313</c:v>
+                  <c:v>0.197592</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -328,7 +390,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$9</c:f>
+              <c:f>Sheet1!$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -337,18 +399,18 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln w="63500"/>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$6:$G$6</c:f>
+              <c:f>Sheet1!$B$5:$G$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
                 <c:pt idx="1">
                   <c:v>5.0</c:v>
                 </c:pt>
@@ -369,27 +431,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$9:$G$9</c:f>
+              <c:f>Sheet1!$B$8:$G$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.719306</c:v>
-                </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.409348</c:v>
+                  <c:v>0.595683</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.327061</c:v>
+                  <c:v>0.42894</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.27093</c:v>
+                  <c:v>0.340305</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.253793</c:v>
+                  <c:v>0.311184</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.261874</c:v>
+                  <c:v>0.313586</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -464,7 +523,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1400"/>
-                  <a:t>Test Error</a:t>
+                  <a:t>Error on Test Set</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -493,6 +552,350 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Naive Bayes and Linear</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Regression Test Errors</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Regression</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="63500"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$16:$M$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="1">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$17:$M$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="1">
+                  <c:v>0.550219</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.375987</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.265187</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.203362</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.197592</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Naïve Bayes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="63500"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$16:$M$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="1">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$18:$M$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="1">
+                  <c:v>0.574947</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.403229</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.326391</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.301076</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.320237</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DraftKings Error</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$16:$M$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="1">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$19:$M$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="1">
+                  <c:v>0.595683</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.42894</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.340305</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.311184</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.313586</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2122434216"/>
+        <c:axId val="-2122432072"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2122434216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Minimum Points Per Game to Be Included In Error Estimate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2122432072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2122432072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Error on Test Set</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2122434216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
@@ -504,7 +907,45 @@
 </chartsheet>
 </file>
 
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="114" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8566930" cy="5815263"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
@@ -853,10 +1294,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -864,7 +1305,7 @@
     <col min="1" max="1" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -881,147 +1322,361 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.30592000000000003</v>
+        <v>0.27983799999999998</v>
       </c>
       <c r="C2">
-        <v>0.30305700000000002</v>
+        <v>0.27818300000000001</v>
       </c>
       <c r="D2">
-        <v>0.30249300000000001</v>
+        <v>0.27794999999999997</v>
       </c>
       <c r="E2">
-        <v>0.30254199999999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>0.27793299999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
-        <v>0.27983799999999998</v>
-      </c>
-      <c r="C3">
-        <v>0.27818300000000001</v>
-      </c>
-      <c r="D3">
-        <v>0.27794999999999997</v>
-      </c>
-      <c r="E3">
-        <v>0.27793299999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4">
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E5">
+        <v>20</v>
+      </c>
+      <c r="F5">
+        <v>30</v>
+      </c>
+      <c r="G5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
       <c r="C6">
-        <v>5</v>
+        <v>0.59417699999999996</v>
       </c>
       <c r="D6">
-        <v>10</v>
+        <v>0.40477099999999999</v>
       </c>
       <c r="E6">
-        <v>20</v>
+        <v>0.27237699999999998</v>
       </c>
       <c r="F6">
-        <v>30</v>
+        <v>0.20224500000000001</v>
       </c>
       <c r="G6">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>0.188836</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B7">
-        <v>0.65547500000000003</v>
-      </c>
       <c r="C7">
-        <v>0.401061</v>
+        <v>0.55021900000000001</v>
       </c>
       <c r="D7">
-        <v>0.30592000000000003</v>
+        <v>0.37598700000000002</v>
       </c>
       <c r="E7">
-        <v>0.21520700000000001</v>
+        <v>0.26518700000000001</v>
       </c>
       <c r="F7">
-        <v>0.170984</v>
+        <v>0.20336199999999999</v>
       </c>
       <c r="G7">
-        <v>0.16054399999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>0.19759199999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>0.59568299999999996</v>
+      </c>
+      <c r="D8">
+        <v>0.42893999999999999</v>
+      </c>
+      <c r="E8">
+        <v>0.34030500000000002</v>
+      </c>
+      <c r="F8">
+        <v>0.31118400000000002</v>
+      </c>
+      <c r="G8">
+        <v>0.31358599999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <f>B12+0.1</f>
+        <v>0.37983800000000001</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ref="C11:D11" si="0">C12+0.1</f>
+        <v>0.37995299999999999</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>0.37893399999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>0.27983799999999998</v>
+      </c>
+      <c r="C12">
+        <v>0.27995300000000001</v>
+      </c>
+      <c r="D12">
+        <v>0.27893400000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" t="s">
         <v>4</v>
       </c>
-      <c r="B8">
-        <v>0.71074400000000004</v>
-      </c>
-      <c r="C8">
-        <v>0.372809</v>
-      </c>
-      <c r="D8">
-        <v>0.27983799999999998</v>
-      </c>
-      <c r="E8">
-        <v>0.20785899999999999</v>
-      </c>
-      <c r="F8">
-        <v>0.17013200000000001</v>
-      </c>
-      <c r="G8">
-        <v>0.16831299999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9">
-        <v>0.719306</v>
-      </c>
-      <c r="C9">
-        <v>0.40934799999999999</v>
-      </c>
-      <c r="D9">
-        <v>0.32706099999999999</v>
-      </c>
-      <c r="E9">
-        <v>0.27093</v>
-      </c>
-      <c r="F9">
-        <v>0.25379299999999999</v>
-      </c>
-      <c r="G9">
-        <v>0.261874</v>
+      <c r="I16">
+        <v>5</v>
+      </c>
+      <c r="J16">
+        <v>10</v>
+      </c>
+      <c r="K16">
+        <v>20</v>
+      </c>
+      <c r="L16">
+        <v>30</v>
+      </c>
+      <c r="M16">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17">
+        <v>25</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17">
+        <v>0.55021900000000001</v>
+      </c>
+      <c r="J17">
+        <v>0.37598700000000002</v>
+      </c>
+      <c r="K17">
+        <v>0.26518700000000001</v>
+      </c>
+      <c r="L17">
+        <v>0.20336199999999999</v>
+      </c>
+      <c r="M17">
+        <v>0.19759199999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18">
+        <v>25</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18">
+        <v>0.57494699999999999</v>
+      </c>
+      <c r="J18">
+        <v>0.403229</v>
+      </c>
+      <c r="K18">
+        <v>0.32639099999999999</v>
+      </c>
+      <c r="L18">
+        <v>0.30107600000000001</v>
+      </c>
+      <c r="M18">
+        <v>0.32023699999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19">
+        <v>25</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>5</v>
+      </c>
+      <c r="I19">
+        <v>0.59568299999999996</v>
+      </c>
+      <c r="J19">
+        <v>0.42893999999999999</v>
+      </c>
+      <c r="K19">
+        <v>0.34030500000000002</v>
+      </c>
+      <c r="L19">
+        <v>0.31118400000000002</v>
+      </c>
+      <c r="M19">
+        <v>0.31358599999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>0.49542999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>0.47017799999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22">
+        <v>11</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>0.42753799999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>10</v>
+      </c>
+      <c r="C23">
+        <v>0.41927599999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24">
+        <v>0.403229</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25">
+        <v>10</v>
+      </c>
+      <c r="C25">
+        <v>0.397397</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26">
+        <v>5</v>
+      </c>
+      <c r="C26">
+        <v>0.390787</v>
       </c>
     </row>
   </sheetData>

</xml_diff>